<commit_message>
Updated the name for checklists
</commit_message>
<xml_diff>
--- a/images/rembi_image_schema_main_v0.1.xlsx
+++ b/images/rembi_image_schema_main_v0.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zef22hak/development/COPO_refactoring/COPO-production/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/providen/Documents/EI/Projects/COPO-schemas/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA898B7-9C37-2F48-A3EC-A45185765A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276FD77B-53B1-804A-95E2-BD7BF17D96E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36860" yWindow="3600" windowWidth="25280" windowHeight="14280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -666,9 +666,6 @@
     <t>version_rembi</t>
   </si>
   <si>
-    <t>REcommended Metadata for Biological Images (REMBI)</t>
-  </si>
-  <si>
     <t>REcommended Metadata for Biological Images (REMBI) provides a way to explain how images have been generated, providing enough context to allow others to interpret them without reference to external sources.</t>
   </si>
   <si>
@@ -1661,6 +1658,9 @@
   </si>
   <si>
     <t>FILE</t>
+  </si>
+  <si>
+    <t>REMBI images</t>
   </si>
 </sst>
 </file>
@@ -2695,7 +2695,7 @@
   </sheetPr>
   <dimension ref="A1:P696"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="G47" sqref="G47"/>
     </sheetView>
@@ -2722,49 +2722,49 @@
   <sheetData>
     <row r="1" spans="1:16" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" s="27" t="s">
         <v>202</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="C1" s="26" t="s">
         <v>203</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="D1" s="70" t="s">
         <v>204</v>
-      </c>
-      <c r="D1" s="70" t="s">
-        <v>205</v>
       </c>
       <c r="E1" s="27" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>504</v>
+      </c>
+      <c r="H1" s="27" t="s">
         <v>206</v>
       </c>
-      <c r="G1" s="27" t="s">
-        <v>505</v>
-      </c>
-      <c r="H1" s="27" t="s">
+      <c r="I1" s="28" t="s">
         <v>207</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="J1" s="29" t="s">
         <v>208</v>
-      </c>
-      <c r="J1" s="29" t="s">
-        <v>209</v>
       </c>
       <c r="K1" s="27" t="s">
         <v>8</v>
       </c>
       <c r="L1" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="M1" s="27" t="s">
         <v>210</v>
       </c>
-      <c r="M1" s="27" t="s">
+      <c r="N1" s="27" t="s">
         <v>211</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="O1" s="28" t="s">
         <v>212</v>
-      </c>
-      <c r="O1" s="28" t="s">
-        <v>213</v>
       </c>
       <c r="P1" s="30" t="s">
         <v>180</v>
@@ -2775,33 +2775,33 @@
         <v>155</v>
       </c>
       <c r="B2" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="C2" s="31" t="s">
         <v>214</v>
       </c>
-      <c r="C2" s="31" t="s">
-        <v>215</v>
-      </c>
       <c r="D2" s="68" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E2" s="31"/>
       <c r="F2" s="32" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G2" s="32"/>
       <c r="H2" s="32"/>
       <c r="I2" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="J2" s="34" t="s">
         <v>217</v>
-      </c>
-      <c r="J2" s="34" t="s">
-        <v>218</v>
       </c>
       <c r="K2" s="31"/>
       <c r="L2" s="31"/>
       <c r="M2" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="N2" s="31" t="s">
         <v>219</v>
-      </c>
-      <c r="N2" s="31" t="s">
-        <v>220</v>
       </c>
       <c r="O2" s="35"/>
       <c r="P2" s="36" t="s">
@@ -2816,34 +2816,34 @@
         <v>6</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E3" s="38"/>
       <c r="F3" s="39" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G3" s="39"/>
       <c r="H3" s="38"/>
       <c r="I3" s="40" t="s">
+        <v>222</v>
+      </c>
+      <c r="J3" s="41" t="s">
         <v>223</v>
       </c>
-      <c r="J3" s="41" t="s">
+      <c r="K3" s="38" t="s">
         <v>224</v>
       </c>
-      <c r="K3" s="38" t="s">
+      <c r="L3" s="42" t="s">
         <v>225</v>
       </c>
-      <c r="L3" s="42" t="s">
-        <v>226</v>
-      </c>
       <c r="M3" s="38" t="s">
+        <v>218</v>
+      </c>
+      <c r="N3" s="38" t="s">
         <v>219</v>
-      </c>
-      <c r="N3" s="38" t="s">
-        <v>220</v>
       </c>
       <c r="O3" s="40"/>
       <c r="P3" s="43" t="s">
@@ -2861,34 +2861,34 @@
         <v>152</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E4" s="42"/>
       <c r="F4" s="39" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G4" s="71"/>
       <c r="H4" s="42"/>
       <c r="I4" s="45" t="s">
+        <v>226</v>
+      </c>
+      <c r="J4" s="46" t="s">
         <v>227</v>
       </c>
-      <c r="J4" s="46" t="s">
+      <c r="K4" s="42" t="s">
+        <v>224</v>
+      </c>
+      <c r="L4" s="42" t="s">
+        <v>225</v>
+      </c>
+      <c r="M4" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N4" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="O4" s="47" t="s">
         <v>228</v>
-      </c>
-      <c r="K4" s="42" t="s">
-        <v>225</v>
-      </c>
-      <c r="L4" s="42" t="s">
-        <v>226</v>
-      </c>
-      <c r="M4" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="N4" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="O4" s="47" t="s">
-        <v>229</v>
       </c>
       <c r="P4" s="43" t="s">
         <v>157</v>
@@ -2902,19 +2902,19 @@
         <v>6</v>
       </c>
       <c r="C5" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D5" s="18" t="s">
         <v>230</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>231</v>
       </c>
       <c r="E5" s="42"/>
       <c r="F5" s="39" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G5" s="71"/>
       <c r="H5" s="42"/>
       <c r="I5" s="45" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J5" s="48">
         <v>46539</v>
@@ -2923,16 +2923,16 @@
         <v>81</v>
       </c>
       <c r="L5" s="42" t="s">
+        <v>232</v>
+      </c>
+      <c r="M5" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N5" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="O5" s="47" t="s">
         <v>233</v>
-      </c>
-      <c r="M5" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="N5" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="O5" s="47" t="s">
-        <v>234</v>
       </c>
       <c r="P5" s="43" t="s">
         <v>157</v>
@@ -2946,33 +2946,33 @@
         <v>6</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E6" s="42"/>
       <c r="F6" s="39" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G6" s="71"/>
       <c r="H6" s="42"/>
       <c r="I6" s="45" t="s">
+        <v>235</v>
+      </c>
+      <c r="J6" s="46" t="s">
         <v>236</v>
-      </c>
-      <c r="J6" s="46" t="s">
-        <v>237</v>
       </c>
       <c r="K6" s="42"/>
       <c r="L6" s="42"/>
       <c r="M6" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N6" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="N6" s="18" t="s">
-        <v>220</v>
-      </c>
       <c r="O6" s="47" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="P6" s="43" t="s">
         <v>157</v>
@@ -2986,33 +2986,33 @@
         <v>6</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E7" s="42"/>
       <c r="F7" s="39" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G7" s="71"/>
       <c r="H7" s="42"/>
       <c r="I7" s="45" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J7" s="46" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K7" s="42"/>
       <c r="L7" s="42"/>
       <c r="M7" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N7" s="49" t="s">
+        <v>239</v>
+      </c>
+      <c r="O7" s="47" t="s">
         <v>240</v>
-      </c>
-      <c r="O7" s="47" t="s">
-        <v>241</v>
       </c>
       <c r="P7" s="43" t="s">
         <v>159</v>
@@ -3026,33 +3026,33 @@
         <v>6</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E8" s="42"/>
       <c r="F8" s="39" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G8" s="71"/>
       <c r="H8" s="42"/>
       <c r="I8" s="45" t="s">
+        <v>242</v>
+      </c>
+      <c r="J8" s="46" t="s">
         <v>243</v>
-      </c>
-      <c r="J8" s="46" t="s">
-        <v>244</v>
       </c>
       <c r="K8" s="42"/>
       <c r="L8" s="42"/>
       <c r="M8" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N8" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="N8" s="18" t="s">
-        <v>220</v>
-      </c>
       <c r="O8" s="47" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="P8" s="43" t="s">
         <v>159</v>
@@ -3066,33 +3066,33 @@
         <v>6</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E9" s="42"/>
       <c r="F9" s="39" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G9" s="71"/>
       <c r="H9" s="42"/>
       <c r="I9" s="45" t="s">
+        <v>246</v>
+      </c>
+      <c r="J9" s="46" t="s">
         <v>247</v>
-      </c>
-      <c r="J9" s="46" t="s">
-        <v>248</v>
       </c>
       <c r="K9" s="42"/>
       <c r="L9" s="42"/>
       <c r="M9" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N9" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="N9" s="18" t="s">
-        <v>220</v>
-      </c>
       <c r="O9" s="47" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="P9" s="43" t="s">
         <v>159</v>
@@ -3106,34 +3106,34 @@
         <v>6</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E10" s="51"/>
       <c r="F10" s="39" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G10" s="72"/>
       <c r="H10" s="51"/>
       <c r="I10" s="52" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J10" s="53">
         <v>1.5</v>
       </c>
       <c r="K10" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="L10" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="L10" s="18" t="s">
-        <v>253</v>
-      </c>
       <c r="M10" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N10" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N10" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O10" s="52"/>
       <c r="P10" s="43" t="s">
@@ -3145,35 +3145,35 @@
         <v>158</v>
       </c>
       <c r="B11" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="C11" s="31" t="s">
         <v>214</v>
       </c>
-      <c r="C11" s="31" t="s">
-        <v>215</v>
-      </c>
       <c r="D11" s="68" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E11" s="31"/>
       <c r="F11" s="32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G11" s="32"/>
       <c r="H11" s="32" t="s">
         <v>155</v>
       </c>
       <c r="I11" s="33" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J11" s="55" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K11" s="31"/>
       <c r="L11" s="31"/>
       <c r="M11" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="N11" s="31" t="s">
         <v>219</v>
-      </c>
-      <c r="N11" s="31" t="s">
-        <v>220</v>
       </c>
       <c r="O11" s="33"/>
       <c r="P11" s="36" t="s">
@@ -3188,17 +3188,17 @@
         <v>6</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F12" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G12" s="56"/>
       <c r="I12" s="12" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J12" s="57">
         <v>12345</v>
@@ -3206,13 +3206,13 @@
       <c r="K12" s="18"/>
       <c r="L12" s="18"/>
       <c r="M12" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N12" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="N12" s="18" t="s">
-        <v>220</v>
-      </c>
       <c r="O12" s="58" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="P12" s="59" t="s">
         <v>157</v>
@@ -3226,31 +3226,31 @@
         <v>6</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D13" s="69" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="F13" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G13" s="56"/>
       <c r="I13" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="J13" s="60" t="s">
         <v>258</v>
-      </c>
-      <c r="J13" s="60" t="s">
-        <v>259</v>
       </c>
       <c r="K13" s="18"/>
       <c r="L13" s="18"/>
       <c r="M13" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N13" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="N13" s="18" t="s">
-        <v>220</v>
-      </c>
       <c r="O13" s="58" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="P13" s="43" t="s">
         <v>157</v>
@@ -3261,35 +3261,35 @@
         <v>160</v>
       </c>
       <c r="B14" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="C14" s="31" t="s">
         <v>214</v>
       </c>
-      <c r="C14" s="31" t="s">
-        <v>215</v>
-      </c>
       <c r="D14" s="18" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E14" s="31"/>
       <c r="F14" s="32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G14" s="32"/>
       <c r="H14" s="32" t="s">
         <v>155</v>
       </c>
       <c r="I14" s="33" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J14" s="34" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K14" s="31"/>
       <c r="L14" s="31"/>
       <c r="M14" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="N14" s="31" t="s">
         <v>219</v>
-      </c>
-      <c r="N14" s="31" t="s">
-        <v>220</v>
       </c>
       <c r="O14" s="35"/>
       <c r="P14" s="61" t="s">
@@ -3304,31 +3304,31 @@
         <v>6</v>
       </c>
       <c r="C15" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>458</v>
+      </c>
+      <c r="F15" s="56" t="s">
         <v>221</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>459</v>
-      </c>
-      <c r="F15" s="56" t="s">
-        <v>222</v>
       </c>
       <c r="G15" s="56"/>
       <c r="I15" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="J15" s="57" t="s">
         <v>261</v>
-      </c>
-      <c r="J15" s="57" t="s">
-        <v>262</v>
       </c>
       <c r="K15" s="18"/>
       <c r="L15" s="18"/>
       <c r="M15" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N15" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="N15" s="18" t="s">
-        <v>220</v>
-      </c>
       <c r="O15" s="58" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="P15" s="43" t="s">
         <v>157</v>
@@ -3342,31 +3342,31 @@
         <v>6</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F16" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G16" s="56"/>
       <c r="I16" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="J16" s="57" t="s">
         <v>264</v>
-      </c>
-      <c r="J16" s="57" t="s">
-        <v>265</v>
       </c>
       <c r="K16" s="18"/>
       <c r="L16" s="18"/>
       <c r="M16" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N16" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="N16" s="18" t="s">
-        <v>220</v>
-      </c>
       <c r="O16" s="58" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="P16" s="43" t="s">
         <v>159</v>
@@ -3380,33 +3380,33 @@
         <v>6</v>
       </c>
       <c r="C17" s="18" t="s">
+        <v>266</v>
+      </c>
+      <c r="D17" s="18" t="s">
         <v>267</v>
       </c>
-      <c r="D17" s="18" t="s">
-        <v>268</v>
-      </c>
       <c r="F17" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G17" s="56"/>
       <c r="I17" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="J17" s="57" t="s">
         <v>269</v>
       </c>
-      <c r="J17" s="57" t="s">
+      <c r="K17" s="18" t="s">
         <v>270</v>
-      </c>
-      <c r="K17" s="18" t="s">
-        <v>271</v>
       </c>
       <c r="L17" s="18"/>
       <c r="M17" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N17" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="N17" s="18" t="s">
-        <v>220</v>
-      </c>
       <c r="O17" s="58" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="P17" s="43" t="s">
         <v>159</v>
@@ -3420,35 +3420,35 @@
         <v>6</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="F18" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G18" s="56"/>
       <c r="I18" s="12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J18" s="57">
         <v>2025</v>
       </c>
       <c r="K18" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="L18" s="18" t="s">
         <v>275</v>
       </c>
-      <c r="L18" s="18" t="s">
+      <c r="M18" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N18" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="O18" s="58" t="s">
         <v>276</v>
-      </c>
-      <c r="M18" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="N18" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="O18" s="58" t="s">
-        <v>277</v>
       </c>
       <c r="P18" s="43" t="s">
         <v>159</v>
@@ -3462,33 +3462,33 @@
         <v>6</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="F19" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G19" s="56"/>
       <c r="I19" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="J19" s="57">
         <v>32726801</v>
       </c>
       <c r="K19" s="18" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L19" s="18"/>
       <c r="M19" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N19" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="N19" s="18" t="s">
-        <v>220</v>
-      </c>
       <c r="O19" s="58" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="P19" s="59" t="s">
         <v>159</v>
@@ -3499,35 +3499,35 @@
         <v>161</v>
       </c>
       <c r="B20" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="C20" s="31" t="s">
         <v>214</v>
       </c>
-      <c r="C20" s="31" t="s">
-        <v>215</v>
-      </c>
       <c r="D20" s="68" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E20" s="31"/>
       <c r="F20" s="32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G20" s="32"/>
       <c r="H20" s="32" t="s">
         <v>155</v>
       </c>
       <c r="I20" s="33" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J20" s="34" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K20" s="31"/>
       <c r="L20" s="31"/>
       <c r="M20" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="N20" s="31" t="s">
         <v>219</v>
-      </c>
-      <c r="N20" s="31" t="s">
-        <v>220</v>
       </c>
       <c r="O20" s="35"/>
       <c r="P20" s="61" t="s">
@@ -3542,26 +3542,26 @@
         <v>6</v>
       </c>
       <c r="C21" s="18" t="s">
+        <v>281</v>
+      </c>
+      <c r="D21" s="18" t="s">
         <v>282</v>
       </c>
-      <c r="D21" s="18" t="s">
-        <v>283</v>
-      </c>
       <c r="F21" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G21" s="56"/>
       <c r="I21" s="12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J21" s="57"/>
       <c r="K21" s="18"/>
       <c r="L21" s="18"/>
       <c r="M21" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N21" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N21" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O21" s="58"/>
       <c r="P21" s="43" t="s">
@@ -3576,26 +3576,26 @@
         <v>6</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F22" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G22" s="56"/>
       <c r="I22" s="12" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J22" s="57"/>
       <c r="K22" s="18"/>
       <c r="L22" s="18"/>
       <c r="M22" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N22" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N22" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O22" s="58"/>
       <c r="P22" s="43" t="s">
@@ -3610,32 +3610,32 @@
         <v>6</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D23" s="69" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F23" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G23" s="56"/>
       <c r="I23" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="J23" s="57" t="s">
         <v>288</v>
       </c>
-      <c r="J23" s="57" t="s">
-        <v>289</v>
-      </c>
       <c r="K23" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="L23" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="L23" s="18" t="s">
-        <v>253</v>
-      </c>
       <c r="M23" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N23" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N23" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O23" s="58"/>
       <c r="P23" s="59" t="s">
@@ -3647,35 +3647,35 @@
         <v>162</v>
       </c>
       <c r="B24" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="C24" s="31" t="s">
         <v>214</v>
       </c>
-      <c r="C24" s="31" t="s">
-        <v>215</v>
-      </c>
       <c r="D24" s="18" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E24" s="31"/>
       <c r="F24" s="32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G24" s="32"/>
       <c r="H24" s="32" t="s">
         <v>155</v>
       </c>
       <c r="I24" s="33" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J24" s="34" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K24" s="31"/>
       <c r="L24" s="31"/>
       <c r="M24" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="N24" s="31" t="s">
         <v>219</v>
-      </c>
-      <c r="N24" s="31" t="s">
-        <v>220</v>
       </c>
       <c r="O24" s="35"/>
       <c r="P24" s="36" t="s">
@@ -3687,33 +3687,33 @@
         <v>162</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C25" s="18" t="s">
+        <v>290</v>
+      </c>
+      <c r="D25" s="18" t="s">
         <v>291</v>
       </c>
-      <c r="D25" s="18" t="s">
+      <c r="F25" s="56" t="s">
+        <v>215</v>
+      </c>
+      <c r="G25" s="56" t="s">
+        <v>505</v>
+      </c>
+      <c r="I25" s="12" t="s">
         <v>292</v>
       </c>
-      <c r="F25" s="56" t="s">
-        <v>216</v>
-      </c>
-      <c r="G25" s="56" t="s">
-        <v>506</v>
-      </c>
-      <c r="I25" s="12" t="s">
+      <c r="J25" s="57" t="s">
         <v>293</v>
-      </c>
-      <c r="J25" s="57" t="s">
-        <v>294</v>
       </c>
       <c r="K25" s="18"/>
       <c r="L25" s="18"/>
       <c r="M25" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N25" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N25" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O25" s="58"/>
       <c r="P25" s="59" t="s">
@@ -3731,25 +3731,25 @@
         <v>4</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F26" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G26" s="56"/>
       <c r="I26" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="J26" s="57" t="s">
         <v>295</v>
-      </c>
-      <c r="J26" s="57" t="s">
-        <v>296</v>
       </c>
       <c r="K26" s="18"/>
       <c r="L26" s="18"/>
       <c r="M26" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N26" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N26" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O26" s="58"/>
       <c r="P26" s="43" t="s">
@@ -3767,23 +3767,23 @@
         <v>152</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F27" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G27" s="56"/>
       <c r="I27" s="12" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="J27" s="57"/>
       <c r="K27" s="18"/>
       <c r="L27" s="18"/>
       <c r="M27" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N27" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N27" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O27" s="58"/>
       <c r="P27" s="43" t="s">
@@ -3795,35 +3795,35 @@
         <v>174</v>
       </c>
       <c r="B28" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="C28" s="31" t="s">
         <v>214</v>
       </c>
-      <c r="C28" s="31" t="s">
-        <v>215</v>
-      </c>
       <c r="D28" s="68" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E28" s="31"/>
       <c r="F28" s="32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G28" s="32"/>
       <c r="H28" s="32" t="s">
         <v>155</v>
       </c>
       <c r="I28" s="33" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J28" s="34" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K28" s="31"/>
       <c r="L28" s="31"/>
       <c r="M28" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="N28" s="31" t="s">
         <v>219</v>
-      </c>
-      <c r="N28" s="31" t="s">
-        <v>220</v>
       </c>
       <c r="O28" s="35"/>
       <c r="P28" s="36" t="s">
@@ -3838,32 +3838,32 @@
         <v>6</v>
       </c>
       <c r="C29" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>473</v>
+      </c>
+      <c r="F29" s="56" t="s">
+        <v>215</v>
+      </c>
+      <c r="G29" s="56" t="s">
+        <v>506</v>
+      </c>
+      <c r="I29" s="12" t="s">
         <v>298</v>
       </c>
-      <c r="D29" s="18" t="s">
-        <v>474</v>
-      </c>
-      <c r="F29" s="56" t="s">
-        <v>216</v>
-      </c>
-      <c r="G29" s="56" t="s">
-        <v>507</v>
-      </c>
-      <c r="I29" s="12" t="s">
+      <c r="J29" s="57" t="s">
         <v>299</v>
-      </c>
-      <c r="J29" s="57" t="s">
-        <v>300</v>
       </c>
       <c r="K29" s="18"/>
       <c r="L29" s="18" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="M29" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N29" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N29" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O29" s="12"/>
       <c r="P29" s="62" t="s">
@@ -3878,30 +3878,30 @@
         <v>6</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F30" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G30" s="56"/>
       <c r="I30" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="J30" s="57" t="s">
         <v>303</v>
-      </c>
-      <c r="J30" s="57" t="s">
-        <v>304</v>
       </c>
       <c r="K30" s="18"/>
       <c r="L30" s="18" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="M30" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N30" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N30" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O30" s="12"/>
       <c r="P30" s="43" t="s">
@@ -3916,31 +3916,31 @@
         <v>6</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F31" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G31" s="56"/>
       <c r="I31" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="J31" s="57" t="s">
         <v>307</v>
-      </c>
-      <c r="J31" s="57" t="s">
-        <v>308</v>
       </c>
       <c r="K31" s="18"/>
       <c r="L31" s="18"/>
       <c r="M31" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N31" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="N31" s="18" t="s">
-        <v>220</v>
-      </c>
       <c r="O31" s="58" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="P31" s="43" t="s">
         <v>159</v>
@@ -3954,29 +3954,29 @@
         <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F32" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G32" s="56"/>
       <c r="I32" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="J32" s="63" t="s">
+        <v>193</v>
+      </c>
+      <c r="M32" s="18" t="s">
         <v>310</v>
       </c>
-      <c r="J32" s="63" t="s">
-        <v>194</v>
-      </c>
-      <c r="M32" s="18" t="s">
+      <c r="N32" s="49" t="s">
+        <v>239</v>
+      </c>
+      <c r="O32" s="58" t="s">
         <v>311</v>
-      </c>
-      <c r="N32" s="49" t="s">
-        <v>240</v>
-      </c>
-      <c r="O32" s="58" t="s">
-        <v>312</v>
       </c>
       <c r="P32" s="43" t="s">
         <v>159</v>
@@ -3990,26 +3990,26 @@
         <v>6</v>
       </c>
       <c r="C33" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="F33" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G33" s="56"/>
       <c r="I33" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="J33" s="63" t="s">
         <v>314</v>
       </c>
-      <c r="J33" s="63" t="s">
-        <v>315</v>
-      </c>
       <c r="M33" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N33" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N33" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="P33" s="43" t="s">
         <v>157</v>
@@ -4023,26 +4023,26 @@
         <v>6</v>
       </c>
       <c r="C34" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="F34" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G34" s="56"/>
       <c r="I34" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="J34" s="63" t="s">
         <v>317</v>
       </c>
-      <c r="J34" s="63" t="s">
-        <v>318</v>
-      </c>
       <c r="M34" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N34" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N34" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="P34" s="43" t="s">
         <v>159</v>
@@ -4056,26 +4056,26 @@
         <v>6</v>
       </c>
       <c r="C35" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F35" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G35" s="56"/>
       <c r="I35" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="J35" s="63" t="s">
         <v>320</v>
       </c>
-      <c r="J35" s="63" t="s">
-        <v>321</v>
-      </c>
       <c r="M35" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N35" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N35" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="P35" s="43" t="s">
         <v>159</v>
@@ -4089,26 +4089,26 @@
         <v>6</v>
       </c>
       <c r="C36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D36" s="69" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F36" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G36" s="56"/>
       <c r="I36" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="J36" s="63" t="s">
         <v>323</v>
       </c>
-      <c r="J36" s="63" t="s">
-        <v>324</v>
-      </c>
       <c r="M36" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N36" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N36" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="P36" s="43" t="s">
         <v>159</v>
@@ -4119,35 +4119,35 @@
         <v>163</v>
       </c>
       <c r="B37" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="C37" s="31" t="s">
         <v>214</v>
       </c>
-      <c r="C37" s="31" t="s">
-        <v>215</v>
-      </c>
       <c r="D37" s="18" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E37" s="31"/>
       <c r="F37" s="32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G37" s="32"/>
       <c r="H37" s="32" t="s">
         <v>155</v>
       </c>
       <c r="I37" s="33" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J37" s="34" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K37" s="31"/>
       <c r="L37" s="31"/>
       <c r="M37" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="N37" s="31" t="s">
         <v>219</v>
-      </c>
-      <c r="N37" s="31" t="s">
-        <v>220</v>
       </c>
       <c r="O37" s="35"/>
       <c r="P37" s="36" t="s">
@@ -4159,33 +4159,33 @@
         <v>163</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C38" s="18" t="s">
+        <v>324</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>481</v>
+      </c>
+      <c r="F38" s="56" t="s">
+        <v>215</v>
+      </c>
+      <c r="G38" s="56" t="s">
+        <v>507</v>
+      </c>
+      <c r="I38" s="12" t="s">
         <v>325</v>
       </c>
-      <c r="D38" s="18" t="s">
-        <v>482</v>
-      </c>
-      <c r="F38" s="56" t="s">
-        <v>216</v>
-      </c>
-      <c r="G38" s="56" t="s">
-        <v>508</v>
-      </c>
-      <c r="I38" s="12" t="s">
+      <c r="J38" s="57" t="s">
         <v>326</v>
-      </c>
-      <c r="J38" s="57" t="s">
-        <v>327</v>
       </c>
       <c r="K38" s="18"/>
       <c r="L38" s="18"/>
       <c r="M38" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N38" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N38" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O38" s="58"/>
       <c r="P38" s="43" t="s">
@@ -4197,36 +4197,36 @@
         <v>163</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F39" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G39" s="56"/>
       <c r="H39" s="56" t="s">
         <v>174</v>
       </c>
       <c r="I39" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="J39" s="57" t="s">
         <v>299</v>
-      </c>
-      <c r="J39" s="57" t="s">
-        <v>300</v>
       </c>
       <c r="K39" s="18"/>
       <c r="L39" s="18" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="M39" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N39" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N39" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O39" s="12"/>
       <c r="P39" s="62" t="s">
@@ -4238,36 +4238,36 @@
         <v>163</v>
       </c>
       <c r="B40" s="25" t="s">
+        <v>327</v>
+      </c>
+      <c r="C40" s="25" t="s">
         <v>328</v>
       </c>
-      <c r="C40" s="25" t="s">
+      <c r="D40" s="18" t="s">
         <v>329</v>
       </c>
-      <c r="D40" s="18" t="s">
-        <v>330</v>
-      </c>
       <c r="F40" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G40" s="56"/>
       <c r="I40" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="J40" s="57" t="s">
         <v>331</v>
-      </c>
-      <c r="J40" s="57" t="s">
-        <v>332</v>
       </c>
       <c r="K40" s="18" t="s">
         <v>109</v>
       </c>
       <c r="L40" s="18"/>
       <c r="M40" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N40" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="N40" s="18" t="s">
-        <v>220</v>
-      </c>
       <c r="O40" s="58" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="P40" s="64" t="s">
         <v>157</v>
@@ -4278,36 +4278,36 @@
         <v>163</v>
       </c>
       <c r="B41" s="25" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C41" s="25" t="s">
+        <v>333</v>
+      </c>
+      <c r="D41" s="18" t="s">
         <v>334</v>
       </c>
-      <c r="D41" s="18" t="s">
-        <v>335</v>
-      </c>
       <c r="F41" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G41" s="56"/>
       <c r="I41" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="J41" s="57" t="s">
         <v>336</v>
-      </c>
-      <c r="J41" s="57" t="s">
-        <v>337</v>
       </c>
       <c r="K41" s="18" t="s">
         <v>111</v>
       </c>
       <c r="L41" s="18"/>
       <c r="M41" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N41" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="N41" s="18" t="s">
-        <v>220</v>
-      </c>
       <c r="O41" s="58" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="P41" s="59" t="s">
         <v>157</v>
@@ -4321,33 +4321,33 @@
         <v>6</v>
       </c>
       <c r="C42" s="18" t="s">
+        <v>338</v>
+      </c>
+      <c r="D42" s="18" t="s">
         <v>339</v>
       </c>
-      <c r="D42" s="18" t="s">
-        <v>340</v>
-      </c>
       <c r="F42" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G42" s="56"/>
       <c r="I42" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="J42" s="65" t="s">
         <v>341</v>
-      </c>
-      <c r="J42" s="65" t="s">
-        <v>342</v>
       </c>
       <c r="K42" s="18" t="s">
         <v>17</v>
       </c>
       <c r="L42" s="18"/>
       <c r="M42" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N42" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="N42" s="18" t="s">
-        <v>220</v>
-      </c>
       <c r="O42" s="58" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="P42" s="43" t="s">
         <v>159</v>
@@ -4361,32 +4361,32 @@
         <v>6</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F43" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G43" s="56"/>
       <c r="I43" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="J43" s="57" t="s">
         <v>345</v>
-      </c>
-      <c r="J43" s="57" t="s">
-        <v>346</v>
       </c>
       <c r="K43" s="18" t="s">
         <v>99</v>
       </c>
       <c r="L43" s="18" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M43" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N43" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N43" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O43" s="58"/>
       <c r="P43" s="43" t="s">
@@ -4401,31 +4401,31 @@
         <v>6</v>
       </c>
       <c r="C44" s="18" t="s">
+        <v>347</v>
+      </c>
+      <c r="D44" s="18" t="s">
         <v>348</v>
       </c>
-      <c r="D44" s="18" t="s">
-        <v>349</v>
-      </c>
       <c r="F44" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G44" s="56"/>
       <c r="I44" s="12" t="s">
+        <v>349</v>
+      </c>
+      <c r="J44" s="66" t="s">
         <v>350</v>
-      </c>
-      <c r="J44" s="66" t="s">
-        <v>351</v>
       </c>
       <c r="K44" s="18"/>
       <c r="L44" s="18"/>
       <c r="M44" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N44" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="N44" s="18" t="s">
-        <v>220</v>
-      </c>
       <c r="O44" s="58" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="P44" s="43" t="s">
         <v>157</v>
@@ -4439,31 +4439,31 @@
         <v>6</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F45" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G45" s="56"/>
       <c r="I45" s="12" t="s">
+        <v>353</v>
+      </c>
+      <c r="J45" s="57" t="s">
         <v>354</v>
-      </c>
-      <c r="J45" s="57" t="s">
-        <v>355</v>
       </c>
       <c r="K45" s="18"/>
       <c r="L45" s="18"/>
       <c r="M45" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N45" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="N45" s="18" t="s">
-        <v>220</v>
-      </c>
       <c r="O45" s="58" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="P45" s="43" t="s">
         <v>159</v>
@@ -4474,35 +4474,35 @@
         <v>164</v>
       </c>
       <c r="B46" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="C46" s="31" t="s">
         <v>214</v>
       </c>
-      <c r="C46" s="31" t="s">
-        <v>215</v>
-      </c>
       <c r="D46" s="68" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E46" s="31"/>
       <c r="F46" s="32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G46" s="32"/>
       <c r="H46" s="32" t="s">
         <v>155</v>
       </c>
       <c r="I46" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="J46" s="34" t="s">
         <v>217</v>
-      </c>
-      <c r="J46" s="34" t="s">
-        <v>218</v>
       </c>
       <c r="K46" s="31"/>
       <c r="L46" s="31"/>
       <c r="M46" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="N46" s="31" t="s">
         <v>219</v>
-      </c>
-      <c r="N46" s="31" t="s">
-        <v>220</v>
       </c>
       <c r="O46" s="35"/>
       <c r="P46" s="36" t="s">
@@ -4514,31 +4514,31 @@
         <v>164</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C47" s="18" t="s">
+        <v>356</v>
+      </c>
+      <c r="D47" s="18" t="s">
         <v>357</v>
       </c>
-      <c r="D47" s="18" t="s">
-        <v>358</v>
-      </c>
       <c r="F47" s="56" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G47" s="56"/>
       <c r="I47" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="J47" s="57" t="s">
         <v>359</v>
-      </c>
-      <c r="J47" s="57" t="s">
-        <v>360</v>
       </c>
       <c r="K47" s="18"/>
       <c r="L47" s="18"/>
       <c r="M47" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N47" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N47" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O47" s="58"/>
       <c r="P47" s="59" t="s">
@@ -4550,41 +4550,41 @@
         <v>164</v>
       </c>
       <c r="B48" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C48" s="18" t="s">
+        <v>360</v>
+      </c>
+      <c r="D48" s="18" t="s">
         <v>361</v>
       </c>
-      <c r="D48" s="18" t="s">
+      <c r="E48" s="18" t="s">
         <v>362</v>
       </c>
-      <c r="E48" s="18" t="s">
-        <v>363</v>
-      </c>
       <c r="F48" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G48" s="56"/>
       <c r="I48" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="J48" s="57" t="s">
         <v>364</v>
-      </c>
-      <c r="J48" s="57" t="s">
-        <v>365</v>
       </c>
       <c r="K48" s="18" t="s">
         <v>113</v>
       </c>
       <c r="L48" s="18" t="s">
+        <v>365</v>
+      </c>
+      <c r="M48" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N48" s="18" t="s">
         <v>366</v>
       </c>
-      <c r="M48" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="N48" s="18" t="s">
+      <c r="O48" s="58" t="s">
         <v>367</v>
-      </c>
-      <c r="O48" s="58" t="s">
-        <v>368</v>
       </c>
       <c r="P48" s="43" t="s">
         <v>157</v>
@@ -4595,41 +4595,41 @@
         <v>164</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C49" s="18" t="s">
+        <v>368</v>
+      </c>
+      <c r="D49" s="18" t="s">
         <v>369</v>
       </c>
-      <c r="D49" s="18" t="s">
-        <v>370</v>
-      </c>
       <c r="E49" s="18" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F49" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G49" s="56"/>
       <c r="I49" s="12" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="J49" s="57">
         <v>8036</v>
       </c>
       <c r="K49" s="31" t="s">
+        <v>371</v>
+      </c>
+      <c r="L49" s="18" t="s">
         <v>372</v>
       </c>
-      <c r="L49" s="18" t="s">
+      <c r="M49" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N49" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="O49" s="58" t="s">
         <v>373</v>
-      </c>
-      <c r="M49" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="N49" s="18" t="s">
-        <v>367</v>
-      </c>
-      <c r="O49" s="58" t="s">
-        <v>374</v>
       </c>
       <c r="P49" s="67" t="s">
         <v>157</v>
@@ -4640,37 +4640,37 @@
         <v>164</v>
       </c>
       <c r="B50" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C50" s="18" t="s">
         <v>2</v>
       </c>
       <c r="D50" s="18" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E50" s="18" t="s">
         <v>2</v>
       </c>
       <c r="F50" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G50" s="56"/>
       <c r="I50" s="12" t="s">
+        <v>375</v>
+      </c>
+      <c r="J50" s="57" t="s">
         <v>376</v>
-      </c>
-      <c r="J50" s="57" t="s">
-        <v>377</v>
       </c>
       <c r="K50" s="18"/>
       <c r="L50" s="18"/>
       <c r="M50" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N50" s="18" t="s">
+        <v>377</v>
+      </c>
+      <c r="O50" s="58" t="s">
         <v>378</v>
-      </c>
-      <c r="O50" s="58" t="s">
-        <v>379</v>
       </c>
       <c r="P50" s="62" t="s">
         <v>157</v>
@@ -4684,28 +4684,28 @@
         <v>6</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D51" s="18" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="F51" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G51" s="56"/>
       <c r="I51" s="12" t="s">
+        <v>380</v>
+      </c>
+      <c r="J51" s="57" t="s">
         <v>381</v>
-      </c>
-      <c r="J51" s="57" t="s">
-        <v>382</v>
       </c>
       <c r="K51" s="18"/>
       <c r="L51" s="18"/>
       <c r="M51" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N51" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N51" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O51" s="58"/>
       <c r="P51" s="62" t="s">
@@ -4720,26 +4720,26 @@
         <v>6</v>
       </c>
       <c r="C52" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F52" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G52" s="56"/>
       <c r="I52" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="J52" s="63" t="s">
         <v>384</v>
       </c>
-      <c r="J52" s="63" t="s">
-        <v>385</v>
-      </c>
       <c r="M52" t="s">
+        <v>218</v>
+      </c>
+      <c r="N52" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N52" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O52" s="58"/>
       <c r="P52" s="43" t="s">
@@ -4757,28 +4757,28 @@
         <v>152</v>
       </c>
       <c r="D53" s="18" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E53" s="18" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F53" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G53" s="56"/>
       <c r="I53" s="12" t="s">
+        <v>386</v>
+      </c>
+      <c r="J53" s="60" t="s">
         <v>387</v>
-      </c>
-      <c r="J53" s="60" t="s">
-        <v>388</v>
       </c>
       <c r="K53" s="18"/>
       <c r="L53" s="18"/>
       <c r="M53" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N53" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N53" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O53" s="58"/>
       <c r="P53" s="43" t="s">
@@ -4793,28 +4793,28 @@
         <v>6</v>
       </c>
       <c r="C54" s="18" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D54" s="18" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F54" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G54" s="56"/>
       <c r="I54" s="12" t="s">
+        <v>389</v>
+      </c>
+      <c r="J54" s="63" t="s">
         <v>390</v>
-      </c>
-      <c r="J54" s="63" t="s">
-        <v>391</v>
       </c>
       <c r="K54" s="18"/>
       <c r="L54" s="18"/>
       <c r="M54" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N54" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N54" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O54" s="58"/>
       <c r="P54" s="43" t="s">
@@ -4829,28 +4829,28 @@
         <v>6</v>
       </c>
       <c r="C55" s="18" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D55" s="18" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F55" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G55" s="56"/>
       <c r="I55" s="12" t="s">
+        <v>392</v>
+      </c>
+      <c r="J55" s="57" t="s">
         <v>393</v>
-      </c>
-      <c r="J55" s="57" t="s">
-        <v>394</v>
       </c>
       <c r="K55" s="18"/>
       <c r="L55" s="18"/>
       <c r="M55" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N55" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N55" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O55" s="58"/>
       <c r="P55" s="43" t="s">
@@ -4865,28 +4865,28 @@
         <v>6</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D56" s="69" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="F56" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G56" s="56"/>
       <c r="I56" s="12" t="s">
+        <v>395</v>
+      </c>
+      <c r="J56" s="57" t="s">
         <v>396</v>
-      </c>
-      <c r="J56" s="57" t="s">
-        <v>397</v>
       </c>
       <c r="K56" s="18"/>
       <c r="L56" s="18"/>
       <c r="M56" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N56" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N56" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O56" s="58"/>
       <c r="P56" s="59" t="s">
@@ -4898,35 +4898,35 @@
         <v>166</v>
       </c>
       <c r="B57" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="C57" s="31" t="s">
         <v>214</v>
       </c>
-      <c r="C57" s="31" t="s">
-        <v>215</v>
-      </c>
       <c r="D57" s="18" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E57" s="31"/>
       <c r="F57" s="32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G57" s="32"/>
       <c r="H57" s="32" t="s">
         <v>155</v>
       </c>
       <c r="I57" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="J57" s="34" t="s">
         <v>217</v>
-      </c>
-      <c r="J57" s="34" t="s">
-        <v>218</v>
       </c>
       <c r="K57" s="31"/>
       <c r="L57" s="31"/>
       <c r="M57" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="N57" s="31" t="s">
         <v>219</v>
-      </c>
-      <c r="N57" s="31" t="s">
-        <v>220</v>
       </c>
       <c r="O57" s="35"/>
       <c r="P57" s="61" t="s">
@@ -4938,34 +4938,34 @@
         <v>166</v>
       </c>
       <c r="B58" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D58" s="18" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="F58" s="56" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G58" s="56"/>
       <c r="H58" s="56" t="s">
         <v>166</v>
       </c>
       <c r="I58" s="12" t="s">
+        <v>398</v>
+      </c>
+      <c r="J58" s="57" t="s">
         <v>399</v>
-      </c>
-      <c r="J58" s="57" t="s">
-        <v>400</v>
       </c>
       <c r="K58" s="18"/>
       <c r="L58" s="18"/>
       <c r="M58" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N58" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N58" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O58" s="12"/>
       <c r="P58" s="43" t="s">
@@ -4977,34 +4977,34 @@
         <v>166</v>
       </c>
       <c r="B59" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C59" s="18" t="s">
+        <v>356</v>
+      </c>
+      <c r="D59" s="18" t="s">
         <v>357</v>
       </c>
-      <c r="D59" s="18" t="s">
-        <v>358</v>
-      </c>
       <c r="F59" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G59" s="56"/>
       <c r="H59" s="73" t="s">
         <v>164</v>
       </c>
       <c r="I59" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="J59" s="57" t="s">
         <v>359</v>
-      </c>
-      <c r="J59" s="57" t="s">
-        <v>360</v>
       </c>
       <c r="K59" s="18"/>
       <c r="L59" s="18"/>
       <c r="M59" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N59" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N59" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O59" s="58"/>
       <c r="P59" s="59" t="s">
@@ -5016,34 +5016,34 @@
         <v>166</v>
       </c>
       <c r="B60" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C60" s="18" t="s">
+        <v>290</v>
+      </c>
+      <c r="D60" s="18" t="s">
         <v>291</v>
       </c>
-      <c r="D60" s="18" t="s">
-        <v>292</v>
-      </c>
       <c r="F60" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G60" s="56"/>
       <c r="H60" s="56" t="s">
         <v>162</v>
       </c>
       <c r="I60" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="J60" s="57" t="s">
         <v>293</v>
-      </c>
-      <c r="J60" s="57" t="s">
-        <v>294</v>
       </c>
       <c r="K60" s="18"/>
       <c r="L60" s="18"/>
       <c r="M60" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N60" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N60" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O60" s="58"/>
       <c r="P60" s="59" t="s">
@@ -5058,28 +5058,28 @@
         <v>6</v>
       </c>
       <c r="C61" s="18" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F61" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G61" s="56"/>
       <c r="I61" s="12" t="s">
+        <v>401</v>
+      </c>
+      <c r="J61" s="60" t="s">
         <v>402</v>
-      </c>
-      <c r="J61" s="60" t="s">
-        <v>403</v>
       </c>
       <c r="K61" s="18"/>
       <c r="L61" s="18"/>
       <c r="M61" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N61" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N61" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O61" s="58"/>
       <c r="P61" s="43" t="s">
@@ -5094,27 +5094,27 @@
         <v>6</v>
       </c>
       <c r="C62" s="18" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D62" s="18" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F62" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G62" s="56"/>
       <c r="I62" s="12" t="s">
+        <v>404</v>
+      </c>
+      <c r="J62" s="60" t="s">
         <v>405</v>
-      </c>
-      <c r="J62" s="60" t="s">
-        <v>406</v>
       </c>
       <c r="L62" s="18"/>
       <c r="M62" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N62" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N62" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O62" s="58"/>
       <c r="P62" s="43" t="s">
@@ -5126,35 +5126,35 @@
         <v>168</v>
       </c>
       <c r="B63" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="C63" s="31" t="s">
         <v>214</v>
       </c>
-      <c r="C63" s="31" t="s">
-        <v>215</v>
-      </c>
       <c r="D63" s="68" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E63" s="31"/>
       <c r="F63" s="32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G63" s="32"/>
       <c r="H63" s="32" t="s">
         <v>155</v>
       </c>
       <c r="I63" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="J63" s="34" t="s">
         <v>217</v>
-      </c>
-      <c r="J63" s="34" t="s">
-        <v>218</v>
       </c>
       <c r="K63" s="31"/>
       <c r="L63" s="31"/>
       <c r="M63" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="N63" s="31" t="s">
         <v>219</v>
-      </c>
-      <c r="N63" s="31" t="s">
-        <v>220</v>
       </c>
       <c r="O63" s="33"/>
       <c r="P63" s="61" t="s">
@@ -5166,33 +5166,33 @@
         <v>168</v>
       </c>
       <c r="B64" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C64" s="18" t="s">
+        <v>406</v>
+      </c>
+      <c r="D64" s="18" t="s">
+        <v>492</v>
+      </c>
+      <c r="F64" s="56" t="s">
+        <v>215</v>
+      </c>
+      <c r="G64" s="56" t="s">
+        <v>508</v>
+      </c>
+      <c r="I64" s="12" t="s">
         <v>407</v>
       </c>
-      <c r="D64" s="18" t="s">
-        <v>493</v>
-      </c>
-      <c r="F64" s="56" t="s">
-        <v>216</v>
-      </c>
-      <c r="G64" s="56" t="s">
-        <v>509</v>
-      </c>
-      <c r="I64" s="12" t="s">
+      <c r="J64" s="57" t="s">
         <v>408</v>
-      </c>
-      <c r="J64" s="57" t="s">
-        <v>409</v>
       </c>
       <c r="K64" s="18"/>
       <c r="L64" s="18"/>
       <c r="M64" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N64" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N64" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O64" s="58"/>
       <c r="P64" s="43" t="s">
@@ -5204,34 +5204,34 @@
         <v>168</v>
       </c>
       <c r="B65" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C65" s="18" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D65" s="18" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="F65" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G65" s="56"/>
       <c r="H65" s="56" t="s">
         <v>166</v>
       </c>
       <c r="I65" s="12" t="s">
+        <v>398</v>
+      </c>
+      <c r="J65" s="57" t="s">
         <v>399</v>
-      </c>
-      <c r="J65" s="57" t="s">
-        <v>400</v>
       </c>
       <c r="K65" s="18"/>
       <c r="L65" s="18"/>
       <c r="M65" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N65" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N65" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O65" s="12"/>
       <c r="P65" s="43" t="s">
@@ -5243,32 +5243,32 @@
         <v>168</v>
       </c>
       <c r="B66" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C66" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D66" s="18" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F66" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G66" s="56"/>
       <c r="I66" s="12" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="J66" s="57"/>
       <c r="K66" s="18"/>
       <c r="L66" s="18"/>
       <c r="M66" s="18" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="N66" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="O66" s="58" t="s">
         <v>412</v>
-      </c>
-      <c r="O66" s="58" t="s">
-        <v>413</v>
       </c>
       <c r="P66" s="43" t="s">
         <v>157</v>
@@ -5282,28 +5282,28 @@
         <v>6</v>
       </c>
       <c r="C67" s="18" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D67" s="18" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="F67" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G67" s="56"/>
       <c r="I67" s="12" t="s">
+        <v>414</v>
+      </c>
+      <c r="J67" s="60" t="s">
         <v>415</v>
-      </c>
-      <c r="J67" s="60" t="s">
-        <v>416</v>
       </c>
       <c r="K67" s="18"/>
       <c r="L67" s="18"/>
       <c r="M67" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N67" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N67" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O67" s="58"/>
       <c r="P67" s="43" t="s">
@@ -5318,28 +5318,28 @@
         <v>6</v>
       </c>
       <c r="C68" s="18" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D68" s="69" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F68" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G68" s="56"/>
       <c r="I68" s="12" t="s">
+        <v>417</v>
+      </c>
+      <c r="J68" s="60" t="s">
         <v>418</v>
-      </c>
-      <c r="J68" s="60" t="s">
-        <v>419</v>
       </c>
       <c r="K68" s="18"/>
       <c r="L68" s="18"/>
       <c r="M68" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N68" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N68" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O68" s="58"/>
       <c r="P68" s="59" t="s">
@@ -5351,35 +5351,35 @@
         <v>170</v>
       </c>
       <c r="B69" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="C69" s="31" t="s">
         <v>214</v>
       </c>
-      <c r="C69" s="31" t="s">
-        <v>215</v>
-      </c>
       <c r="D69" s="18" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E69" s="31"/>
       <c r="F69" s="32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G69" s="32"/>
       <c r="H69" s="32" t="s">
         <v>155</v>
       </c>
       <c r="I69" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="J69" s="55" t="s">
         <v>217</v>
-      </c>
-      <c r="J69" s="55" t="s">
-        <v>218</v>
       </c>
       <c r="K69" s="31"/>
       <c r="L69" s="31"/>
       <c r="M69" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="N69" s="31" t="s">
         <v>219</v>
-      </c>
-      <c r="N69" s="31" t="s">
-        <v>220</v>
       </c>
       <c r="O69" s="33"/>
       <c r="P69" s="36" t="s">
@@ -5391,34 +5391,34 @@
         <v>170</v>
       </c>
       <c r="B70" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C70" s="18" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D70" s="18" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F70" s="56" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G70" s="56" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H70" s="56"/>
       <c r="I70" s="12" t="s">
+        <v>420</v>
+      </c>
+      <c r="J70" s="57" t="s">
         <v>421</v>
-      </c>
-      <c r="J70" s="57" t="s">
-        <v>422</v>
       </c>
       <c r="K70" s="18"/>
       <c r="L70" s="18"/>
       <c r="M70" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N70" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N70" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O70" s="12"/>
       <c r="P70" s="43" t="s">
@@ -5430,34 +5430,34 @@
         <v>170</v>
       </c>
       <c r="B71" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C71" s="18" t="s">
+        <v>290</v>
+      </c>
+      <c r="D71" s="18" t="s">
         <v>291</v>
       </c>
-      <c r="D71" s="18" t="s">
-        <v>292</v>
-      </c>
       <c r="F71" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G71" s="56"/>
       <c r="H71" s="56" t="s">
         <v>162</v>
       </c>
       <c r="I71" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="J71" s="57" t="s">
         <v>293</v>
-      </c>
-      <c r="J71" s="57" t="s">
-        <v>294</v>
       </c>
       <c r="K71" s="18"/>
       <c r="L71" s="18"/>
       <c r="M71" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N71" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N71" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O71" s="58"/>
       <c r="P71" s="59" t="s">
@@ -5472,28 +5472,28 @@
         <v>6</v>
       </c>
       <c r="C72" s="18" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D72" s="18" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="F72" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G72" s="56"/>
       <c r="I72" s="12" t="s">
+        <v>423</v>
+      </c>
+      <c r="J72" s="60" t="s">
         <v>424</v>
-      </c>
-      <c r="J72" s="60" t="s">
-        <v>425</v>
       </c>
       <c r="K72" s="18"/>
       <c r="L72" s="18"/>
       <c r="M72" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N72" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N72" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O72" s="12"/>
       <c r="P72" s="43" t="s">
@@ -5505,35 +5505,35 @@
         <v>172</v>
       </c>
       <c r="B73" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="C73" s="31" t="s">
         <v>214</v>
       </c>
-      <c r="C73" s="31" t="s">
-        <v>215</v>
-      </c>
       <c r="D73" s="68" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E73" s="31"/>
       <c r="F73" s="32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G73" s="32"/>
       <c r="H73" s="32" t="s">
         <v>155</v>
       </c>
       <c r="I73" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="J73" s="34" t="s">
         <v>217</v>
-      </c>
-      <c r="J73" s="34" t="s">
-        <v>218</v>
       </c>
       <c r="K73" s="31"/>
       <c r="L73" s="31"/>
       <c r="M73" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="N73" s="31" t="s">
         <v>219</v>
-      </c>
-      <c r="N73" s="31" t="s">
-        <v>220</v>
       </c>
       <c r="O73" s="33"/>
       <c r="P73" s="61" t="s">
@@ -5545,33 +5545,33 @@
         <v>172</v>
       </c>
       <c r="B74" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C74" s="18" t="s">
+        <v>425</v>
+      </c>
+      <c r="D74" s="18" t="s">
+        <v>498</v>
+      </c>
+      <c r="F74" s="56" t="s">
+        <v>215</v>
+      </c>
+      <c r="G74" s="56" t="s">
+        <v>510</v>
+      </c>
+      <c r="I74" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="D74" s="18" t="s">
-        <v>499</v>
-      </c>
-      <c r="F74" s="56" t="s">
-        <v>216</v>
-      </c>
-      <c r="G74" s="56" t="s">
-        <v>511</v>
-      </c>
-      <c r="I74" s="12" t="s">
+      <c r="J74" s="57" t="s">
         <v>427</v>
-      </c>
-      <c r="J74" s="57" t="s">
-        <v>428</v>
       </c>
       <c r="K74" s="18"/>
       <c r="L74" s="18"/>
       <c r="M74" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N74" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N74" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O74" s="12"/>
       <c r="P74" s="43" t="s">
@@ -5583,34 +5583,34 @@
         <v>172</v>
       </c>
       <c r="B75" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C75" s="18" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D75" s="18" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F75" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G75" s="56"/>
       <c r="H75" s="56" t="s">
         <v>170</v>
       </c>
       <c r="I75" s="12" t="s">
+        <v>420</v>
+      </c>
+      <c r="J75" s="57" t="s">
         <v>421</v>
-      </c>
-      <c r="J75" s="57" t="s">
-        <v>422</v>
       </c>
       <c r="K75" s="18"/>
       <c r="L75" s="18"/>
       <c r="M75" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N75" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N75" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O75" s="12"/>
       <c r="P75" s="43" t="s">
@@ -5625,28 +5625,28 @@
         <v>6</v>
       </c>
       <c r="C76" s="18" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D76" s="18" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F76" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G76" s="56"/>
       <c r="I76" s="12" t="s">
+        <v>429</v>
+      </c>
+      <c r="J76" s="57" t="s">
         <v>430</v>
-      </c>
-      <c r="J76" s="57" t="s">
-        <v>431</v>
       </c>
       <c r="K76" s="18"/>
       <c r="L76" s="18"/>
       <c r="M76" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N76" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N76" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O76" s="12"/>
       <c r="P76" s="43" t="s">
@@ -5661,26 +5661,26 @@
         <v>6</v>
       </c>
       <c r="C77" s="18" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D77" s="18" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F77" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G77" s="56"/>
       <c r="I77" s="12" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="J77" s="57"/>
       <c r="K77" s="18"/>
       <c r="L77" s="18"/>
       <c r="M77" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N77" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N77" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O77" s="12"/>
       <c r="P77" s="43" t="s">
@@ -5695,26 +5695,26 @@
         <v>6</v>
       </c>
       <c r="C78" s="12" t="s">
+        <v>433</v>
+      </c>
+      <c r="D78" s="69" t="s">
         <v>434</v>
       </c>
-      <c r="D78" s="69" t="s">
-        <v>435</v>
-      </c>
       <c r="F78" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G78" s="56"/>
       <c r="I78" s="12" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="J78" s="57"/>
       <c r="K78" s="18"/>
       <c r="L78" s="18"/>
       <c r="M78" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N78" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N78" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O78" s="12"/>
       <c r="P78" s="43" t="s">
@@ -5726,35 +5726,35 @@
         <v>176</v>
       </c>
       <c r="B79" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="C79" s="31" t="s">
         <v>214</v>
       </c>
-      <c r="C79" s="31" t="s">
-        <v>215</v>
-      </c>
       <c r="D79" s="18" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E79" s="31"/>
       <c r="F79" s="32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G79" s="32"/>
       <c r="H79" s="32" t="s">
         <v>155</v>
       </c>
       <c r="I79" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="J79" s="34" t="s">
         <v>217</v>
-      </c>
-      <c r="J79" s="34" t="s">
-        <v>218</v>
       </c>
       <c r="K79" s="31"/>
       <c r="L79" s="31"/>
       <c r="M79" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="N79" s="31" t="s">
         <v>219</v>
-      </c>
-      <c r="N79" s="31" t="s">
-        <v>220</v>
       </c>
       <c r="O79" s="33"/>
       <c r="P79" s="61" t="s">
@@ -5766,37 +5766,37 @@
         <v>176</v>
       </c>
       <c r="B80" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C80" s="18" t="s">
+        <v>436</v>
+      </c>
+      <c r="D80" s="18" t="s">
         <v>437</v>
       </c>
-      <c r="D80" s="18" t="s">
+      <c r="F80" s="56" t="s">
+        <v>215</v>
+      </c>
+      <c r="G80" s="56" t="s">
+        <v>511</v>
+      </c>
+      <c r="I80" s="12" t="s">
         <v>438</v>
       </c>
-      <c r="F80" s="56" t="s">
-        <v>216</v>
-      </c>
-      <c r="G80" s="56" t="s">
-        <v>512</v>
-      </c>
-      <c r="I80" s="12" t="s">
+      <c r="J80" s="57" t="s">
         <v>439</v>
-      </c>
-      <c r="J80" s="57" t="s">
-        <v>440</v>
       </c>
       <c r="K80" s="18" t="s">
         <v>11</v>
       </c>
       <c r="L80" s="18" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="M80" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N80" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N80" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O80" s="12"/>
       <c r="P80" s="62" t="s">
@@ -5808,34 +5808,34 @@
         <v>176</v>
       </c>
       <c r="B81" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C81" s="18" t="s">
+        <v>290</v>
+      </c>
+      <c r="D81" s="18" t="s">
         <v>291</v>
       </c>
-      <c r="D81" s="18" t="s">
-        <v>292</v>
-      </c>
       <c r="F81" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G81" s="56"/>
       <c r="H81" s="56" t="s">
         <v>162</v>
       </c>
       <c r="I81" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="J81" s="57" t="s">
         <v>293</v>
-      </c>
-      <c r="J81" s="57" t="s">
-        <v>294</v>
       </c>
       <c r="K81" s="18"/>
       <c r="L81" s="18"/>
       <c r="M81" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N81" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N81" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O81" s="58"/>
       <c r="P81" s="59" t="s">
@@ -5850,33 +5850,33 @@
         <v>6</v>
       </c>
       <c r="C82" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D82" s="18" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F82" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G82" s="56"/>
       <c r="H82" s="56" t="s">
         <v>174</v>
       </c>
       <c r="I82" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="J82" s="57" t="s">
         <v>299</v>
-      </c>
-      <c r="J82" s="57" t="s">
-        <v>300</v>
       </c>
       <c r="K82" s="18"/>
       <c r="L82" s="18" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="M82" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N82" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N82" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O82" s="12"/>
       <c r="P82" s="62" t="s">
@@ -5891,28 +5891,28 @@
         <v>6</v>
       </c>
       <c r="C83" s="18" t="s">
+        <v>441</v>
+      </c>
+      <c r="D83" s="18" t="s">
         <v>442</v>
       </c>
-      <c r="D83" s="18" t="s">
-        <v>443</v>
-      </c>
       <c r="F83" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G83" s="56"/>
       <c r="I83" s="12" t="s">
+        <v>443</v>
+      </c>
+      <c r="J83" s="57" t="s">
         <v>444</v>
-      </c>
-      <c r="J83" s="57" t="s">
-        <v>445</v>
       </c>
       <c r="K83" s="18"/>
       <c r="L83" s="18"/>
       <c r="M83" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N83" s="18" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="O83" s="12"/>
       <c r="P83" s="43" t="s">
@@ -5927,30 +5927,30 @@
         <v>6</v>
       </c>
       <c r="C84" s="18" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D84" s="18" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F84" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G84" s="56"/>
       <c r="I84" s="12" t="s">
+        <v>447</v>
+      </c>
+      <c r="J84" s="57" t="s">
         <v>448</v>
-      </c>
-      <c r="J84" s="57" t="s">
-        <v>449</v>
       </c>
       <c r="K84" s="18"/>
       <c r="L84" s="18" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="M84" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N84" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N84" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="O84" s="12"/>
       <c r="P84" s="43" t="s">
@@ -5965,26 +5965,26 @@
         <v>6</v>
       </c>
       <c r="C85" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D85" s="18" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F85" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G85" s="56"/>
       <c r="I85" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="J85" s="63" t="s">
         <v>452</v>
       </c>
-      <c r="J85" s="63" t="s">
-        <v>453</v>
-      </c>
       <c r="M85" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N85" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N85" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="P85" s="43" t="s">
         <v>159</v>
@@ -5998,32 +5998,32 @@
         <v>6</v>
       </c>
       <c r="C86" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D86" s="18" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F86" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G86" s="56"/>
       <c r="I86" s="8" t="s">
+        <v>454</v>
+      </c>
+      <c r="J86" s="63" t="s">
         <v>455</v>
       </c>
-      <c r="J86" s="63" t="s">
+      <c r="K86" t="s">
         <v>456</v>
       </c>
-      <c r="K86" t="s">
+      <c r="L86" t="s">
         <v>457</v>
       </c>
-      <c r="L86" t="s">
-        <v>458</v>
-      </c>
       <c r="M86" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N86" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="N86" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="P86" s="43" t="s">
         <v>159</v>
@@ -9293,84 +9293,84 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>183</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>184</v>
       </c>
       <c r="C1" s="23"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="B2" s="25" t="s">
         <v>185</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="B3" s="25" t="s">
         <v>187</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B4" s="25" t="s">
         <v>189</v>
-      </c>
-      <c r="B4" s="25" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="B5" s="25" t="s">
         <v>191</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="B6" s="25" t="s">
         <v>193</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="B7" s="25" t="s">
         <v>195</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="25" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="25" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="25" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="25" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -9385,7 +9385,9 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9418,10 +9420,10 @@
         <v>180</v>
       </c>
       <c r="B2" t="s">
+        <v>512</v>
+      </c>
+      <c r="C2" t="s">
         <v>181</v>
-      </c>
-      <c r="C2" t="s">
-        <v>182</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Removed error messages where the corresponding regex field  is empty
</commit_message>
<xml_diff>
--- a/images/rembi_image_schema_main_v0.1.xlsx
+++ b/images/rembi_image_schema_main_v0.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/providen/Documents/EI/Projects/COPO-schemas/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276FD77B-53B1-804A-95E2-BD7BF17D96E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC7E24F-2976-5249-890F-5C7A7376B0B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="512">
   <si>
     <t>copo_name</t>
   </si>
@@ -1023,9 +1023,6 @@
     <t>ANN123</t>
   </si>
   <si>
-    <t>Missing or malformed 'annotation_id'. Must be alphanumeric.</t>
-  </si>
-  <si>
     <t>annotation_overview</t>
   </si>
   <si>
@@ -1035,9 +1032,6 @@
     <t>Cell nuclei marked using DAPI staining.</t>
   </si>
   <si>
-    <t>annotation_overview' is required and must not exceed 255 characters.</t>
-  </si>
-  <si>
     <t>file_type</t>
   </si>
   <si>
@@ -1237,9 +1231,6 @@
   </si>
   <si>
     <t>^[0-9]+$</t>
-  </si>
-  <si>
-    <t>It must be numbers</t>
   </si>
   <si>
     <t>http://rs.tdwg.org/dwc/terms/taxonID</t>
@@ -1471,9 +1462,6 @@
     <t>z-stack flattening</t>
   </si>
   <si>
-    <t>transformations' must be a pipe symbol (|) separated list.</t>
-  </si>
-  <si>
     <t>spatial_information</t>
   </si>
   <si>
@@ -1661,6 +1649,15 @@
   </si>
   <si>
     <t>REMBI images</t>
+  </si>
+  <si>
+    <t>Invalid DOI format. Expected something like '10.xxxx/xxxxx'</t>
+  </si>
+  <si>
+    <t>Value must contain only digits (0–9) and be between 1 and 8 digits long with no spaces, no letters and no punctuation.</t>
+  </si>
+  <si>
+    <t>Value must be digits (0–9) only.</t>
   </si>
 </sst>
 </file>
@@ -2169,7 +2166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2388,6 +2385,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2695,9 +2693,9 @@
   </sheetPr>
   <dimension ref="A1:P696"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L82" sqref="L82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2740,7 +2738,7 @@
         <v>205</v>
       </c>
       <c r="G1" s="27" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="H1" s="27" t="s">
         <v>206</v>
@@ -2819,7 +2817,7 @@
         <v>220</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="E3" s="38"/>
       <c r="F3" s="39" t="s">
@@ -2861,7 +2859,7 @@
         <v>152</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="E4" s="42"/>
       <c r="F4" s="39" t="s">
@@ -2949,7 +2947,7 @@
         <v>234</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="E6" s="42"/>
       <c r="F6" s="39" t="s">
@@ -2989,7 +2987,7 @@
         <v>182</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="E7" s="42"/>
       <c r="F7" s="39" t="s">
@@ -3029,7 +3027,7 @@
         <v>241</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="E8" s="42"/>
       <c r="F8" s="39" t="s">
@@ -3069,7 +3067,7 @@
         <v>245</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="E9" s="42"/>
       <c r="F9" s="39" t="s">
@@ -3109,7 +3107,7 @@
         <v>249</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="E10" s="51"/>
       <c r="F10" s="39" t="s">
@@ -3191,7 +3189,7 @@
         <v>205</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="F12" s="56" t="s">
         <v>221</v>
@@ -3229,7 +3227,7 @@
         <v>256</v>
       </c>
       <c r="D13" s="69" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="F13" s="56" t="s">
         <v>221</v>
@@ -3307,7 +3305,7 @@
         <v>220</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="F15" s="56" t="s">
         <v>221</v>
@@ -3345,7 +3343,7 @@
         <v>262</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="F16" s="56" t="s">
         <v>221</v>
@@ -3398,7 +3396,9 @@
       <c r="K17" s="18" t="s">
         <v>270</v>
       </c>
-      <c r="L17" s="18"/>
+      <c r="L17" s="18" t="s">
+        <v>509</v>
+      </c>
       <c r="M17" s="18" t="s">
         <v>218</v>
       </c>
@@ -3423,7 +3423,7 @@
         <v>272</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="F18" s="56" t="s">
         <v>221</v>
@@ -3465,7 +3465,7 @@
         <v>277</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="F19" s="56" t="s">
         <v>221</v>
@@ -3480,7 +3480,9 @@
       <c r="K19" s="18" t="s">
         <v>279</v>
       </c>
-      <c r="L19" s="18"/>
+      <c r="L19" s="18" t="s">
+        <v>510</v>
+      </c>
       <c r="M19" s="18" t="s">
         <v>218</v>
       </c>
@@ -3579,7 +3581,7 @@
         <v>284</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="F22" s="56" t="s">
         <v>221</v>
@@ -3613,7 +3615,7 @@
         <v>286</v>
       </c>
       <c r="D23" s="69" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="F23" s="56" t="s">
         <v>221</v>
@@ -3699,7 +3701,7 @@
         <v>215</v>
       </c>
       <c r="G25" s="56" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="I25" s="12" t="s">
         <v>292</v>
@@ -3731,7 +3733,7 @@
         <v>4</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="F26" s="56" t="s">
         <v>221</v>
@@ -3767,7 +3769,7 @@
         <v>152</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="F27" s="56" t="s">
         <v>221</v>
@@ -3841,13 +3843,13 @@
         <v>297</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="F29" s="56" t="s">
         <v>215</v>
       </c>
       <c r="G29" s="56" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="I29" s="12" t="s">
         <v>298</v>
@@ -3856,9 +3858,7 @@
         <v>299</v>
       </c>
       <c r="K29" s="18"/>
-      <c r="L29" s="18" t="s">
-        <v>300</v>
-      </c>
+      <c r="L29" s="18"/>
       <c r="M29" s="18" t="s">
         <v>218</v>
       </c>
@@ -3878,25 +3878,23 @@
         <v>6</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="F30" s="56" t="s">
         <v>221</v>
       </c>
       <c r="G30" s="56"/>
       <c r="I30" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="J30" s="57" t="s">
         <v>302</v>
       </c>
-      <c r="J30" s="57" t="s">
-        <v>303</v>
-      </c>
       <c r="K30" s="18"/>
-      <c r="L30" s="18" t="s">
-        <v>304</v>
-      </c>
+      <c r="L30" s="18"/>
       <c r="M30" s="18" t="s">
         <v>218</v>
       </c>
@@ -3916,20 +3914,20 @@
         <v>6</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="F31" s="56" t="s">
         <v>221</v>
       </c>
       <c r="G31" s="56"/>
       <c r="I31" s="12" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="J31" s="57" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="K31" s="18"/>
       <c r="L31" s="18"/>
@@ -3940,7 +3938,7 @@
         <v>219</v>
       </c>
       <c r="O31" s="58" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="P31" s="43" t="s">
         <v>159</v>
@@ -3957,26 +3955,26 @@
         <v>183</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="F32" s="56" t="s">
         <v>221</v>
       </c>
       <c r="G32" s="56"/>
       <c r="I32" s="8" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="J32" s="63" t="s">
         <v>193</v>
       </c>
       <c r="M32" s="18" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="N32" s="49" t="s">
         <v>239</v>
       </c>
       <c r="O32" s="58" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="P32" s="43" t="s">
         <v>159</v>
@@ -3990,20 +3988,20 @@
         <v>6</v>
       </c>
       <c r="C33" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="F33" s="56" t="s">
         <v>221</v>
       </c>
       <c r="G33" s="56"/>
       <c r="I33" s="8" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="J33" s="63" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="M33" s="18" t="s">
         <v>218</v>
@@ -4023,20 +4021,20 @@
         <v>6</v>
       </c>
       <c r="C34" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="F34" s="56" t="s">
         <v>221</v>
       </c>
       <c r="G34" s="56"/>
       <c r="I34" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="J34" s="63" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="M34" s="18" t="s">
         <v>218</v>
@@ -4056,20 +4054,20 @@
         <v>6</v>
       </c>
       <c r="C35" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="F35" s="56" t="s">
         <v>221</v>
       </c>
       <c r="G35" s="56"/>
       <c r="I35" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="J35" s="63" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="M35" s="18" t="s">
         <v>218</v>
@@ -4089,20 +4087,20 @@
         <v>6</v>
       </c>
       <c r="C36" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D36" s="69" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="F36" s="56" t="s">
         <v>221</v>
       </c>
       <c r="G36" s="56"/>
       <c r="I36" s="8" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="J36" s="63" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="M36" s="18" t="s">
         <v>218</v>
@@ -4162,22 +4160,22 @@
         <v>213</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="F38" s="56" t="s">
         <v>215</v>
       </c>
       <c r="G38" s="56" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="I38" s="12" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="J38" s="57" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="K38" s="18"/>
       <c r="L38" s="18"/>
@@ -4203,7 +4201,7 @@
         <v>297</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="F39" s="56" t="s">
         <v>221</v>
@@ -4219,9 +4217,7 @@
         <v>299</v>
       </c>
       <c r="K39" s="18"/>
-      <c r="L39" s="18" t="s">
-        <v>300</v>
-      </c>
+      <c r="L39" s="18"/>
       <c r="M39" s="18" t="s">
         <v>218</v>
       </c>
@@ -4238,23 +4234,23 @@
         <v>163</v>
       </c>
       <c r="B40" s="25" t="s">
+        <v>325</v>
+      </c>
+      <c r="C40" s="25" t="s">
+        <v>326</v>
+      </c>
+      <c r="D40" s="18" t="s">
         <v>327</v>
-      </c>
-      <c r="C40" s="25" t="s">
-        <v>328</v>
-      </c>
-      <c r="D40" s="18" t="s">
-        <v>329</v>
       </c>
       <c r="F40" s="56" t="s">
         <v>221</v>
       </c>
       <c r="G40" s="56"/>
       <c r="I40" s="12" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="J40" s="57" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="K40" s="18" t="s">
         <v>109</v>
@@ -4267,7 +4263,7 @@
         <v>219</v>
       </c>
       <c r="O40" s="58" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="P40" s="64" t="s">
         <v>157</v>
@@ -4278,23 +4274,23 @@
         <v>163</v>
       </c>
       <c r="B41" s="25" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C41" s="25" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F41" s="56" t="s">
         <v>221</v>
       </c>
       <c r="G41" s="56"/>
       <c r="I41" s="12" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="J41" s="57" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="K41" s="18" t="s">
         <v>111</v>
@@ -4307,7 +4303,7 @@
         <v>219</v>
       </c>
       <c r="O41" s="58" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="P41" s="59" t="s">
         <v>157</v>
@@ -4321,20 +4317,20 @@
         <v>6</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F42" s="56" t="s">
         <v>221</v>
       </c>
       <c r="G42" s="56"/>
       <c r="I42" s="12" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="J42" s="65" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="K42" s="18" t="s">
         <v>17</v>
@@ -4347,7 +4343,7 @@
         <v>219</v>
       </c>
       <c r="O42" s="58" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="P42" s="43" t="s">
         <v>159</v>
@@ -4361,26 +4357,26 @@
         <v>6</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="F43" s="56" t="s">
         <v>221</v>
       </c>
       <c r="G43" s="56"/>
       <c r="I43" s="12" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="J43" s="57" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="K43" s="18" t="s">
         <v>99</v>
       </c>
       <c r="L43" s="18" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="M43" s="18" t="s">
         <v>218</v>
@@ -4401,20 +4397,20 @@
         <v>6</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="F44" s="56" t="s">
         <v>221</v>
       </c>
       <c r="G44" s="56"/>
       <c r="I44" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="J44" s="66" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="K44" s="18"/>
       <c r="L44" s="18"/>
@@ -4425,7 +4421,7 @@
         <v>219</v>
       </c>
       <c r="O44" s="58" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="P44" s="43" t="s">
         <v>157</v>
@@ -4439,20 +4435,20 @@
         <v>6</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="F45" s="56" t="s">
         <v>221</v>
       </c>
       <c r="G45" s="56"/>
       <c r="I45" s="12" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="J45" s="57" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="K45" s="18"/>
       <c r="L45" s="18"/>
@@ -4463,7 +4459,7 @@
         <v>219</v>
       </c>
       <c r="O45" s="58" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="P45" s="43" t="s">
         <v>159</v>
@@ -4517,20 +4513,20 @@
         <v>213</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="F47" s="56" t="s">
         <v>215</v>
       </c>
       <c r="G47" s="56"/>
       <c r="I47" s="12" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="J47" s="57" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="K47" s="18"/>
       <c r="L47" s="18"/>
@@ -4553,38 +4549,38 @@
         <v>213</v>
       </c>
       <c r="C48" s="18" t="s">
+        <v>358</v>
+      </c>
+      <c r="D48" s="18" t="s">
+        <v>359</v>
+      </c>
+      <c r="E48" s="18" t="s">
         <v>360</v>
-      </c>
-      <c r="D48" s="18" t="s">
-        <v>361</v>
-      </c>
-      <c r="E48" s="18" t="s">
-        <v>362</v>
       </c>
       <c r="F48" s="56" t="s">
         <v>221</v>
       </c>
       <c r="G48" s="56"/>
       <c r="I48" s="12" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="J48" s="57" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="K48" s="18" t="s">
         <v>113</v>
       </c>
       <c r="L48" s="18" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="M48" s="18" t="s">
         <v>218</v>
       </c>
       <c r="N48" s="18" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="O48" s="58" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="P48" s="43" t="s">
         <v>157</v>
@@ -4598,38 +4594,38 @@
         <v>213</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D49" s="18" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E49" s="18" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="F49" s="56" t="s">
         <v>221</v>
       </c>
       <c r="G49" s="56"/>
       <c r="I49" s="12" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="J49" s="57">
         <v>8036</v>
       </c>
       <c r="K49" s="31" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="L49" s="18" t="s">
-        <v>372</v>
+        <v>511</v>
       </c>
       <c r="M49" s="18" t="s">
         <v>218</v>
       </c>
       <c r="N49" s="18" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="O49" s="58" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="P49" s="67" t="s">
         <v>157</v>
@@ -4646,7 +4642,7 @@
         <v>2</v>
       </c>
       <c r="D50" s="18" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="E50" s="18" t="s">
         <v>2</v>
@@ -4656,10 +4652,10 @@
       </c>
       <c r="G50" s="56"/>
       <c r="I50" s="12" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="J50" s="57" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="K50" s="18"/>
       <c r="L50" s="18"/>
@@ -4667,10 +4663,10 @@
         <v>218</v>
       </c>
       <c r="N50" s="18" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="O50" s="58" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="P50" s="62" t="s">
         <v>157</v>
@@ -4684,20 +4680,20 @@
         <v>6</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D51" s="18" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="F51" s="56" t="s">
         <v>221</v>
       </c>
       <c r="G51" s="56"/>
       <c r="I51" s="12" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="J51" s="57" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="K51" s="18"/>
       <c r="L51" s="18"/>
@@ -4720,20 +4716,20 @@
         <v>6</v>
       </c>
       <c r="C52" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="F52" s="56" t="s">
         <v>221</v>
       </c>
       <c r="G52" s="56"/>
       <c r="I52" s="8" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="J52" s="63" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="M52" t="s">
         <v>218</v>
@@ -4757,20 +4753,20 @@
         <v>152</v>
       </c>
       <c r="D53" s="18" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="E53" s="18" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="F53" s="56" t="s">
         <v>221</v>
       </c>
       <c r="G53" s="56"/>
       <c r="I53" s="12" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="J53" s="60" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="K53" s="18"/>
       <c r="L53" s="18"/>
@@ -4793,20 +4789,20 @@
         <v>6</v>
       </c>
       <c r="C54" s="18" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D54" s="18" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="F54" s="56" t="s">
         <v>221</v>
       </c>
       <c r="G54" s="56"/>
       <c r="I54" s="12" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="J54" s="63" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="K54" s="18"/>
       <c r="L54" s="18"/>
@@ -4829,20 +4825,20 @@
         <v>6</v>
       </c>
       <c r="C55" s="18" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D55" s="18" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="F55" s="56" t="s">
         <v>221</v>
       </c>
       <c r="G55" s="56"/>
       <c r="I55" s="12" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="J55" s="57" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="K55" s="18"/>
       <c r="L55" s="18"/>
@@ -4865,20 +4861,20 @@
         <v>6</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="D56" s="69" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="F56" s="56" t="s">
         <v>221</v>
       </c>
       <c r="G56" s="56"/>
       <c r="I56" s="12" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="J56" s="57" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="K56" s="18"/>
       <c r="L56" s="18"/>
@@ -4941,10 +4937,10 @@
         <v>213</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="D58" s="18" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="F58" s="56" t="s">
         <v>215</v>
@@ -4954,10 +4950,10 @@
         <v>166</v>
       </c>
       <c r="I58" s="12" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="J58" s="57" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="K58" s="18"/>
       <c r="L58" s="18"/>
@@ -4980,10 +4976,10 @@
         <v>213</v>
       </c>
       <c r="C59" s="18" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D59" s="18" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="F59" s="56" t="s">
         <v>221</v>
@@ -4993,10 +4989,10 @@
         <v>164</v>
       </c>
       <c r="I59" s="12" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="J59" s="57" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="K59" s="18"/>
       <c r="L59" s="18"/>
@@ -5058,20 +5054,20 @@
         <v>6</v>
       </c>
       <c r="C61" s="18" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="F61" s="56" t="s">
         <v>221</v>
       </c>
       <c r="G61" s="56"/>
       <c r="I61" s="12" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="J61" s="60" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="K61" s="18"/>
       <c r="L61" s="18"/>
@@ -5094,20 +5090,20 @@
         <v>6</v>
       </c>
       <c r="C62" s="18" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D62" s="18" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="F62" s="56" t="s">
         <v>221</v>
       </c>
       <c r="G62" s="56"/>
       <c r="I62" s="12" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="J62" s="60" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="L62" s="18"/>
       <c r="M62" s="18" t="s">
@@ -5169,22 +5165,22 @@
         <v>213</v>
       </c>
       <c r="C64" s="18" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D64" s="18" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="F64" s="56" t="s">
         <v>215</v>
       </c>
       <c r="G64" s="56" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="I64" s="12" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="J64" s="57" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="K64" s="18"/>
       <c r="L64" s="18"/>
@@ -5207,10 +5203,10 @@
         <v>213</v>
       </c>
       <c r="C65" s="18" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="D65" s="18" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="F65" s="56" t="s">
         <v>221</v>
@@ -5220,10 +5216,10 @@
         <v>166</v>
       </c>
       <c r="I65" s="12" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="J65" s="57" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="K65" s="18"/>
       <c r="L65" s="18"/>
@@ -5246,29 +5242,29 @@
         <v>213</v>
       </c>
       <c r="C66" s="18" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D66" s="18" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="F66" s="56" t="s">
         <v>221</v>
       </c>
       <c r="G66" s="56"/>
       <c r="I66" s="12" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="J66" s="57"/>
       <c r="K66" s="18"/>
       <c r="L66" s="18"/>
       <c r="M66" s="18" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="N66" s="18" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="O66" s="58" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="P66" s="43" t="s">
         <v>157</v>
@@ -5282,20 +5278,20 @@
         <v>6</v>
       </c>
       <c r="C67" s="18" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="D67" s="18" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="F67" s="56" t="s">
         <v>221</v>
       </c>
       <c r="G67" s="56"/>
       <c r="I67" s="12" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="J67" s="60" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="K67" s="18"/>
       <c r="L67" s="18"/>
@@ -5318,20 +5314,20 @@
         <v>6</v>
       </c>
       <c r="C68" s="18" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="D68" s="69" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="F68" s="56" t="s">
         <v>221</v>
       </c>
       <c r="G68" s="56"/>
       <c r="I68" s="12" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="J68" s="60" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="K68" s="18"/>
       <c r="L68" s="18"/>
@@ -5394,23 +5390,23 @@
         <v>213</v>
       </c>
       <c r="C70" s="18" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="D70" s="18" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="F70" s="56" t="s">
         <v>215</v>
       </c>
       <c r="G70" s="56" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="H70" s="56"/>
       <c r="I70" s="12" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="J70" s="57" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="K70" s="18"/>
       <c r="L70" s="18"/>
@@ -5472,20 +5468,20 @@
         <v>6</v>
       </c>
       <c r="C72" s="18" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="D72" s="18" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="F72" s="56" t="s">
         <v>221</v>
       </c>
       <c r="G72" s="56"/>
       <c r="I72" s="12" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="J72" s="60" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="K72" s="18"/>
       <c r="L72" s="18"/>
@@ -5548,22 +5544,22 @@
         <v>213</v>
       </c>
       <c r="C74" s="18" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="D74" s="18" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="F74" s="56" t="s">
         <v>215</v>
       </c>
       <c r="G74" s="56" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="I74" s="12" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="J74" s="57" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="K74" s="18"/>
       <c r="L74" s="18"/>
@@ -5586,10 +5582,10 @@
         <v>213</v>
       </c>
       <c r="C75" s="18" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="D75" s="18" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="F75" s="56" t="s">
         <v>221</v>
@@ -5599,10 +5595,10 @@
         <v>170</v>
       </c>
       <c r="I75" s="12" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="J75" s="57" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="K75" s="18"/>
       <c r="L75" s="18"/>
@@ -5625,20 +5621,20 @@
         <v>6</v>
       </c>
       <c r="C76" s="18" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="D76" s="18" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="F76" s="56" t="s">
         <v>221</v>
       </c>
       <c r="G76" s="56"/>
       <c r="I76" s="12" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="J76" s="57" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="K76" s="18"/>
       <c r="L76" s="18"/>
@@ -5661,17 +5657,17 @@
         <v>6</v>
       </c>
       <c r="C77" s="18" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="D77" s="18" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="F77" s="56" t="s">
         <v>221</v>
       </c>
       <c r="G77" s="56"/>
       <c r="I77" s="12" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="J77" s="57"/>
       <c r="K77" s="18"/>
@@ -5695,17 +5691,17 @@
         <v>6</v>
       </c>
       <c r="C78" s="12" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D78" s="69" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="F78" s="56" t="s">
         <v>221</v>
       </c>
       <c r="G78" s="56"/>
       <c r="I78" s="12" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="J78" s="57"/>
       <c r="K78" s="18"/>
@@ -5769,28 +5765,28 @@
         <v>213</v>
       </c>
       <c r="C80" s="18" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D80" s="18" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="F80" s="56" t="s">
         <v>215</v>
       </c>
       <c r="G80" s="56" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="I80" s="12" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="J80" s="57" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="K80" s="18" t="s">
         <v>11</v>
       </c>
       <c r="L80" s="18" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="M80" s="18" t="s">
         <v>218</v>
@@ -5853,7 +5849,7 @@
         <v>297</v>
       </c>
       <c r="D82" s="18" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="F82" s="56" t="s">
         <v>221</v>
@@ -5869,9 +5865,7 @@
         <v>299</v>
       </c>
       <c r="K82" s="18"/>
-      <c r="L82" s="18" t="s">
-        <v>300</v>
-      </c>
+      <c r="L82" s="18"/>
       <c r="M82" s="18" t="s">
         <v>218</v>
       </c>
@@ -5891,20 +5885,20 @@
         <v>6</v>
       </c>
       <c r="C83" s="18" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="D83" s="18" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="F83" s="56" t="s">
         <v>221</v>
       </c>
       <c r="G83" s="56"/>
       <c r="I83" s="12" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="J83" s="57" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="K83" s="18"/>
       <c r="L83" s="18"/>
@@ -5912,7 +5906,7 @@
         <v>218</v>
       </c>
       <c r="N83" s="18" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="O83" s="12"/>
       <c r="P83" s="43" t="s">
@@ -5927,25 +5921,23 @@
         <v>6</v>
       </c>
       <c r="C84" s="18" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="D84" s="18" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="F84" s="56" t="s">
         <v>221</v>
       </c>
       <c r="G84" s="56"/>
       <c r="I84" s="12" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="J84" s="57" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="K84" s="18"/>
-      <c r="L84" s="18" t="s">
-        <v>449</v>
-      </c>
+      <c r="L84" s="18"/>
       <c r="M84" s="18" t="s">
         <v>218</v>
       </c>
@@ -5965,20 +5957,20 @@
         <v>6</v>
       </c>
       <c r="C85" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="D85" s="18" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="F85" s="56" t="s">
         <v>221</v>
       </c>
       <c r="G85" s="56"/>
       <c r="I85" s="8" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="J85" s="63" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="M85" s="18" t="s">
         <v>218</v>
@@ -5998,26 +5990,26 @@
         <v>6</v>
       </c>
       <c r="C86" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="D86" s="18" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="F86" s="56" t="s">
         <v>221</v>
       </c>
       <c r="G86" s="56"/>
       <c r="I86" s="8" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="J86" s="63" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="K86" t="s">
-        <v>456</v>
-      </c>
-      <c r="L86" t="s">
-        <v>457</v>
+        <v>452</v>
+      </c>
+      <c r="L86" s="74" t="s">
+        <v>453</v>
       </c>
       <c r="M86" s="18" t="s">
         <v>218</v>
@@ -9385,7 +9377,7 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -9420,7 +9412,7 @@
         <v>180</v>
       </c>
       <c r="B2" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="C2" t="s">
         <v>181</v>

</xml_diff>